<commit_message>
Creating a new build
</commit_message>
<xml_diff>
--- a/LAGC.xlsx
+++ b/LAGC.xlsx
@@ -3,8 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Hoja 2" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Capturando" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Concatenado" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
   <si>
     <t>No.</t>
   </si>
@@ -20,125 +20,170 @@
     <t>Abreviatura</t>
   </si>
   <si>
+    <t>Apellido</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>Categoría</t>
+  </si>
+  <si>
+    <t>Mtro.</t>
+  </si>
+  <si>
+    <t>Aguilar Pérez</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>Profesor Asistente "B"</t>
+  </si>
+  <si>
+    <t>Castañeda Gonzalez</t>
+  </si>
+  <si>
+    <t>Carlos Alberto</t>
+  </si>
+  <si>
+    <t>https://mti.cucea.udg.mx/?q=mtro-carlos-alberto-castaneda-gonzalez#overlay-context=mtro-jose-guadalupe-morales-montelongo%3Fq%3Dmtro-jose-guadalupe-morales-montelongo</t>
+  </si>
+  <si>
+    <t>Profesor Externo</t>
+  </si>
+  <si>
+    <t>Dra.</t>
+  </si>
+  <si>
+    <t>Correa Cortéz</t>
+  </si>
+  <si>
+    <t>Maria Esmeralda</t>
+  </si>
+  <si>
+    <t>Profesor Titular "B"</t>
+  </si>
+  <si>
+    <t>Cruz Herrera</t>
+  </si>
+  <si>
+    <t>Ma. Hidalia</t>
+  </si>
+  <si>
+    <t>Profesor Asignatura</t>
+  </si>
+  <si>
+    <t>Mtra.</t>
+  </si>
+  <si>
+    <t>Cruz Ornelas</t>
+  </si>
+  <si>
+    <t>Larisa</t>
+  </si>
+  <si>
+    <t>Dr.</t>
+  </si>
+  <si>
+    <t>Dávalos García</t>
+  </si>
+  <si>
+    <t>Sergio Roberto</t>
+  </si>
+  <si>
+    <t>Profesor Investigador Asociado "A"</t>
+  </si>
+  <si>
+    <t>Hugo Enrique</t>
+  </si>
+  <si>
+    <t>Torres Ruvalcaba</t>
+  </si>
+  <si>
+    <t>https://mti.cucea.udg.mx/?q=mtro-hugo-enrique-torres-ruvalcaba#overlay-context=hugo-enrique-torres-ruvalcaba%3Fq%3Dhugo-enrique-torres-ruvalcaba</t>
+  </si>
+  <si>
+    <t>Profesor Asignatura "B"</t>
+  </si>
+  <si>
+    <t>Ledezma Padilla</t>
+  </si>
+  <si>
+    <t>Mónica Elizabeth</t>
+  </si>
+  <si>
+    <t>Profesor Investigador Asociado "B"</t>
+  </si>
+  <si>
+    <t>Maciel Arellano</t>
+  </si>
+  <si>
+    <t>Ma. Del Rocio</t>
+  </si>
+  <si>
+    <t>https://mti.cucea.udg.mx/?q=dra-ma-del-rocio-maciel-arellano#overlay-context=</t>
+  </si>
+  <si>
+    <t>Profesor Investigador Titular "A"</t>
+  </si>
+  <si>
+    <t>Meda Campaña</t>
+  </si>
+  <si>
+    <t>María Elena</t>
+  </si>
+  <si>
+    <t>https://mti.cucea.udg.mx/?q=dra-maria-elena-meda-campana#overlay-context=dra-ma-del-rocio-maciel-arellano%3Fq%3Ddra-ma-del-rocio-maciel-arellano</t>
+  </si>
+  <si>
+    <t>Profesor Investigador Titular "C"</t>
+  </si>
+  <si>
+    <t>Morales Montelongo</t>
+  </si>
+  <si>
+    <t>José Guadalupe</t>
+  </si>
+  <si>
+    <t>https://mti.cucea.udg.mx/?q=mtro-jose-guadalupe-morales-montelongo#overlay-context=mtro-hugo-enrique-torres-ruvalcaba%3Fq%3Dmtro-hugo-enrique-torres-ruvalcaba</t>
+  </si>
+  <si>
+    <t>Profesor Titular "A"</t>
+  </si>
+  <si>
+    <t>Retamoza Vega</t>
+  </si>
+  <si>
+    <t>Patricia del Rosario</t>
+  </si>
+  <si>
+    <t>Profesor de Tiempo Completo Asociado "C"</t>
+  </si>
+  <si>
+    <t>Reynoso Gómez</t>
+  </si>
+  <si>
+    <t>Blanca Lorena</t>
+  </si>
+  <si>
+    <t>https://mti.cucea.udg.mx/?q=dra-blanca-lorena-reynoso-gomez#overlay-context=practica%3Fq%3Dpractica</t>
+  </si>
+  <si>
+    <t>Profesor Docente Asociado "B"</t>
+  </si>
+  <si>
     <t>Profesor</t>
-  </si>
-  <si>
-    <t>link</t>
-  </si>
-  <si>
-    <t>Categoría</t>
-  </si>
-  <si>
-    <t>Dra.</t>
-  </si>
-  <si>
-    <t>Blanca Lorena Reynoso Gómez</t>
-  </si>
-  <si>
-    <t>https://mti.cucea.udg.mx/?q=dra-blanca-lorena-reynoso-gomez#overlay-context=practica%3Fq%3Dpractica</t>
-  </si>
-  <si>
-    <t>Profesor Docente Asociado "B"</t>
-  </si>
-  <si>
-    <t>Mtro.</t>
-  </si>
-  <si>
-    <t>Carlos Alberto Castañeda Gonzalez</t>
-  </si>
-  <si>
-    <t>https://mti.cucea.udg.mx/?q=mtro-carlos-alberto-castaneda-gonzalez#overlay-context=mtro-jose-guadalupe-morales-montelongo%3Fq%3Dmtro-jose-guadalupe-morales-montelongo</t>
-  </si>
-  <si>
-    <t>Profesor Externo</t>
-  </si>
-  <si>
-    <t>Cruz Herrera Ma. Hidalia</t>
-  </si>
-  <si>
-    <t>Profesor Asignatura</t>
-  </si>
-  <si>
-    <t>José Guadalupe Morales Montelongo</t>
-  </si>
-  <si>
-    <t>https://mti.cucea.udg.mx/?q=mtro-jose-guadalupe-morales-montelongo#overlay-context=mtro-hugo-enrique-torres-ruvalcaba%3Fq%3Dmtro-hugo-enrique-torres-ruvalcaba</t>
-  </si>
-  <si>
-    <t>Profesor Titular "A"</t>
-  </si>
-  <si>
-    <t>Larisa Cruz Ornelas</t>
-  </si>
-  <si>
-    <t>Ma. Del Rocio Maciel Arellano</t>
-  </si>
-  <si>
-    <t>https://mti.cucea.udg.mx/?q=dra-ma-del-rocio-maciel-arellano#overlay-context=</t>
-  </si>
-  <si>
-    <t>Profesor Investigador Titular "A"</t>
-  </si>
-  <si>
-    <t>María Elena Meda Campaña</t>
-  </si>
-  <si>
-    <t>https://mti.cucea.udg.mx/?q=dra-maria-elena-meda-campana#overlay-context=dra-ma-del-rocio-maciel-arellano%3Fq%3Ddra-ma-del-rocio-maciel-arellano</t>
-  </si>
-  <si>
-    <t>Profesor Investigador Titular "C"</t>
-  </si>
-  <si>
-    <t>Maria Esmeralda Correa Cortéz</t>
-  </si>
-  <si>
-    <t>Profesor Titular "B"</t>
-  </si>
-  <si>
-    <t>Mtra.</t>
-  </si>
-  <si>
-    <t>Mónica Elizabeth Ledezma Padilla</t>
-  </si>
-  <si>
-    <t>Profesor Investigador Asociado "B"</t>
-  </si>
-  <si>
-    <t>Patricia del Rosario Retamoza Vega</t>
-  </si>
-  <si>
-    <t>Profesor de Tiempo Completo Asociado "C"</t>
-  </si>
-  <si>
-    <t>Pedro Aguilar Pérez</t>
-  </si>
-  <si>
-    <t>Profesor Asistente "B"</t>
-  </si>
-  <si>
-    <t>Dr.</t>
-  </si>
-  <si>
-    <t>Sergio Roberto Dávalos García</t>
-  </si>
-  <si>
-    <t>Profesor Investigador Asociado "A"</t>
-  </si>
-  <si>
-    <t>Torres Ruvalcaba Hugo Enrique</t>
-  </si>
-  <si>
-    <t>https://mti.cucea.udg.mx/?q=mtro-hugo-enrique-torres-ruvalcaba#overlay-context=hugo-enrique-torres-ruvalcaba%3Fq%3Dhugo-enrique-torres-ruvalcaba</t>
-  </si>
-  <si>
-    <t>Profesor Asignatura "B"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -159,6 +204,10 @@
       <name val="Inherit"/>
     </font>
     <font>
+      <color rgb="FF336F9D"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -170,10 +219,25 @@
     </font>
     <font>
       <u/>
+      <color rgb="FF336F9D"/>
+      <name val="Open Sans"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF336F9D"/>
+      <name val="&quot;docs-Open Sans&quot;"/>
+    </font>
+    <font>
+      <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font>
+      <u/>
+      <color rgb="FF444444"/>
+      <name val="Inherit"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,6 +248,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF16325C"/>
         <bgColor rgb="FF16325C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -207,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -223,8 +293,8 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -232,7 +302,22 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
   </cellXfs>
@@ -456,9 +541,10 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="3.75"/>
-    <col customWidth="1" min="2" max="2" width="11.13"/>
-    <col customWidth="1" min="3" max="4" width="34.75"/>
-    <col customWidth="1" min="5" max="5" width="46.63"/>
+    <col customWidth="1" min="2" max="2" width="6.63"/>
+    <col customWidth="1" min="3" max="4" width="31.13"/>
+    <col customWidth="1" min="5" max="5" width="34.75"/>
+    <col customWidth="1" min="6" max="6" width="46.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -477,22 +563,26 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2">
         <v>1.0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -500,16 +590,19 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="4" t="s">
         <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4">
@@ -517,14 +610,17 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5">
@@ -532,16 +628,17 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6">
@@ -549,48 +646,54 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2">
         <v>6.0</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>21</v>
+      <c r="B7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2">
         <v>7.0</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>24</v>
+      <c r="B8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9">
@@ -598,14 +701,17 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10">
@@ -613,14 +719,19 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11">
@@ -628,14 +739,19 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12">
@@ -643,71 +759,87 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="2" t="s">
-        <v>33</v>
+        <v>43</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2">
         <v>12.0</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>36</v>
+      <c r="B13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2">
         <v>13.0</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>39</v>
+      <c r="B14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="8"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16">
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="2"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" location="overlay-context=practica%3Fq%3Dpractica" ref="D2"/>
-    <hyperlink r:id="rId2" location="overlay-context=mtro-jose-guadalupe-morales-montelongo%3Fq%3Dmtro-jose-guadalupe-morales-montelongo" ref="D3"/>
-    <hyperlink r:id="rId3" location="overlay-context=mtro-hugo-enrique-torres-ruvalcaba%3Fq%3Dmtro-hugo-enrique-torres-ruvalcaba" ref="D5"/>
-    <hyperlink r:id="rId4" location="overlay-context=" ref="D7"/>
-    <hyperlink r:id="rId5" location="overlay-context=dra-ma-del-rocio-maciel-arellano%3Fq%3Ddra-ma-del-rocio-maciel-arellano" ref="D8"/>
-    <hyperlink r:id="rId6" ref="C13"/>
-    <hyperlink r:id="rId7" location="overlay-context=hugo-enrique-torres-ruvalcaba%3Fq%3Dhugo-enrique-torres-ruvalcaba" ref="C14"/>
-    <hyperlink r:id="rId8" location="overlay-context=hugo-enrique-torres-ruvalcaba%3Fq%3Dhugo-enrique-torres-ruvalcaba" ref="D14"/>
+    <hyperlink r:id="rId1" location="overlay-context=mtro-jose-guadalupe-morales-montelongo%3Fq%3Dmtro-jose-guadalupe-morales-montelongo" ref="E3"/>
+    <hyperlink r:id="rId2" ref="C7"/>
+    <hyperlink r:id="rId3" ref="D7"/>
+    <hyperlink r:id="rId4" location="overlay-context=hugo-enrique-torres-ruvalcaba%3Fq%3Dhugo-enrique-torres-ruvalcaba" ref="C8"/>
+    <hyperlink r:id="rId5" location="overlay-context=hugo-enrique-torres-ruvalcaba%3Fq%3Dhugo-enrique-torres-ruvalcaba" ref="D8"/>
+    <hyperlink r:id="rId6" location="overlay-context=hugo-enrique-torres-ruvalcaba%3Fq%3Dhugo-enrique-torres-ruvalcaba" ref="E8"/>
+    <hyperlink r:id="rId7" location="overlay-context=" ref="E10"/>
+    <hyperlink r:id="rId8" location="overlay-context=dra-ma-del-rocio-maciel-arellano%3Fq%3Ddra-ma-del-rocio-maciel-arellano" ref="E11"/>
+    <hyperlink r:id="rId9" location="overlay-context=mtro-hugo-enrique-torres-ruvalcaba%3Fq%3Dmtro-hugo-enrique-torres-ruvalcaba" ref="E12"/>
+    <hyperlink r:id="rId10" location="overlay-context=practica%3Fq%3Dpractica" ref="E14"/>
   </hyperlinks>
-  <drawing r:id="rId9"/>
+  <drawing r:id="rId11"/>
 </worksheet>
 </file>
 
@@ -722,7 +854,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="38.88"/>
-    <col customWidth="1" min="3" max="3" width="39.13"/>
+    <col customWidth="1" min="3" max="4" width="39.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -730,10 +862,11 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>54</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2">
@@ -741,12 +874,16 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="3" t="str">
-        <f>CONCATENATE('Hoja 1'!B2, " ", 'Hoja 1'!C2)</f>
-        <v>Dra. Blanca Lorena Reynoso Gómez</v>
-      </c>
-      <c r="C2" s="2" t="str">
-        <f>'Hoja 1'!E2</f>
-        <v>Profesor Docente Asociado "B"</v>
+        <f>CONCATENATE(Capturando!B2, " ", Capturando!C2, " ", Capturando!D2)</f>
+        <v>Mtro. Aguilar Pérez Pedro</v>
+      </c>
+      <c r="C2" s="12" t="str">
+        <f>Capturando!E2</f>
+        <v/>
+      </c>
+      <c r="D2" s="2" t="str">
+        <f>Capturando!F2</f>
+        <v>Profesor Asistente "B"</v>
       </c>
     </row>
     <row r="3">
@@ -754,11 +891,15 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="3" t="str">
-        <f>CONCATENATE('Hoja 1'!B3, " ", 'Hoja 1'!C3)</f>
-        <v>Mtro. Carlos Alberto Castañeda Gonzalez</v>
-      </c>
-      <c r="C3" s="2" t="str">
-        <f>'Hoja 1'!E3</f>
+        <f>CONCATENATE(Capturando!B3, " ", Capturando!C3, " ", Capturando!D3)</f>
+        <v>Mtro. Castañeda Gonzalez Carlos Alberto</v>
+      </c>
+      <c r="C3" s="13" t="str">
+        <f>Capturando!E3</f>
+        <v>https://mti.cucea.udg.mx/?q=mtro-carlos-alberto-castaneda-gonzalez#overlay-context=mtro-jose-guadalupe-morales-montelongo%3Fq%3Dmtro-jose-guadalupe-morales-montelongo</v>
+      </c>
+      <c r="D3" s="2" t="str">
+        <f>Capturando!F3</f>
         <v>Profesor Externo</v>
       </c>
     </row>
@@ -767,12 +908,16 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="3" t="str">
-        <f>CONCATENATE('Hoja 1'!B4, " ", 'Hoja 1'!C4)</f>
-        <v>Dra. Cruz Herrera Ma. Hidalia</v>
-      </c>
-      <c r="C4" s="2" t="str">
-        <f>'Hoja 1'!E4</f>
-        <v>Profesor Asignatura</v>
+        <f>CONCATENATE(Capturando!B4, " ", Capturando!C4, " ", Capturando!D4)</f>
+        <v>Dra. Correa Cortéz Maria Esmeralda</v>
+      </c>
+      <c r="C4" s="12" t="str">
+        <f>Capturando!E4</f>
+        <v/>
+      </c>
+      <c r="D4" s="2" t="str">
+        <f>Capturando!F4</f>
+        <v>Profesor Titular "B"</v>
       </c>
     </row>
     <row r="5">
@@ -780,12 +925,16 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="3" t="str">
-        <f>CONCATENATE('Hoja 1'!B5, " ", 'Hoja 1'!C5)</f>
-        <v>Mtro. José Guadalupe Morales Montelongo</v>
-      </c>
-      <c r="C5" s="2" t="str">
-        <f>'Hoja 1'!E5</f>
-        <v>Profesor Titular "A"</v>
+        <f>CONCATENATE(Capturando!B5, " ", Capturando!C5, " ", Capturando!D5)</f>
+        <v>Dra. Cruz Herrera Ma. Hidalia</v>
+      </c>
+      <c r="C5" s="12" t="str">
+        <f>Capturando!E5</f>
+        <v/>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f>Capturando!F5</f>
+        <v>Profesor Asignatura</v>
       </c>
     </row>
     <row r="6">
@@ -793,11 +942,15 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="3" t="str">
-        <f>CONCATENATE('Hoja 1'!B6, " ", 'Hoja 1'!C6)</f>
-        <v>Mtro. Larisa Cruz Ornelas</v>
-      </c>
-      <c r="C6" s="2" t="str">
-        <f>'Hoja 1'!E6</f>
+        <f>CONCATENATE(Capturando!B6, " ", Capturando!C6, " ", Capturando!D6)</f>
+        <v>Mtra. Cruz Ornelas Larisa</v>
+      </c>
+      <c r="C6" s="12" t="str">
+        <f>Capturando!E6</f>
+        <v/>
+      </c>
+      <c r="D6" s="2" t="str">
+        <f>Capturando!F6</f>
         <v>Profesor Externo</v>
       </c>
     </row>
@@ -806,12 +959,16 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="3" t="str">
-        <f>CONCATENATE('Hoja 1'!B7, " ", 'Hoja 1'!C7)</f>
-        <v>Dra. Ma. Del Rocio Maciel Arellano</v>
-      </c>
-      <c r="C7" s="2" t="str">
-        <f>'Hoja 1'!E7</f>
-        <v>Profesor Investigador Titular "A"</v>
+        <f>CONCATENATE(Capturando!B7, " ", Capturando!C7, " ", Capturando!D7)</f>
+        <v>Dr. Dávalos García Sergio Roberto</v>
+      </c>
+      <c r="C7" s="12" t="str">
+        <f>Capturando!E7</f>
+        <v/>
+      </c>
+      <c r="D7" s="2" t="str">
+        <f>Capturando!F7</f>
+        <v>Profesor Investigador Asociado "A"</v>
       </c>
     </row>
     <row r="8">
@@ -819,12 +976,16 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="3" t="str">
-        <f>CONCATENATE('Hoja 1'!B8, " ", 'Hoja 1'!C8)</f>
-        <v>Dra. María Elena Meda Campaña</v>
-      </c>
-      <c r="C8" s="2" t="str">
-        <f>'Hoja 1'!E8</f>
-        <v>Profesor Investigador Titular "C"</v>
+        <f>CONCATENATE(Capturando!B8, " ", Capturando!C8, " ", Capturando!D8)</f>
+        <v>Mtro. Hugo Enrique Torres Ruvalcaba</v>
+      </c>
+      <c r="C8" s="13" t="str">
+        <f>Capturando!E8</f>
+        <v>https://mti.cucea.udg.mx/?q=mtro-hugo-enrique-torres-ruvalcaba#overlay-context=hugo-enrique-torres-ruvalcaba%3Fq%3Dhugo-enrique-torres-ruvalcaba</v>
+      </c>
+      <c r="D8" s="2" t="str">
+        <f>Capturando!F8</f>
+        <v>Profesor Asignatura "B"</v>
       </c>
     </row>
     <row r="9">
@@ -832,12 +993,16 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="3" t="str">
-        <f>CONCATENATE('Hoja 1'!B9, " ", 'Hoja 1'!C9)</f>
-        <v>Dra. Maria Esmeralda Correa Cortéz</v>
-      </c>
-      <c r="C9" s="2" t="str">
-        <f>'Hoja 1'!E9</f>
-        <v>Profesor Titular "B"</v>
+        <f>CONCATENATE(Capturando!B9, " ", Capturando!C9, " ", Capturando!D9)</f>
+        <v>Mtra. Ledezma Padilla Mónica Elizabeth</v>
+      </c>
+      <c r="C9" s="12" t="str">
+        <f>Capturando!E9</f>
+        <v/>
+      </c>
+      <c r="D9" s="2" t="str">
+        <f>Capturando!F9</f>
+        <v>Profesor Investigador Asociado "B"</v>
       </c>
     </row>
     <row r="10">
@@ -845,12 +1010,16 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="3" t="str">
-        <f>CONCATENATE('Hoja 1'!B10, " ", 'Hoja 1'!C10)</f>
-        <v>Mtra. Mónica Elizabeth Ledezma Padilla</v>
-      </c>
-      <c r="C10" s="2" t="str">
-        <f>'Hoja 1'!E10</f>
-        <v>Profesor Investigador Asociado "B"</v>
+        <f>CONCATENATE(Capturando!B10, " ", Capturando!C10, " ", Capturando!D10)</f>
+        <v>Dra. Maciel Arellano Ma. Del Rocio</v>
+      </c>
+      <c r="C10" s="13" t="str">
+        <f>Capturando!E10</f>
+        <v>https://mti.cucea.udg.mx/?q=dra-ma-del-rocio-maciel-arellano#overlay-context=</v>
+      </c>
+      <c r="D10" s="2" t="str">
+        <f>Capturando!F10</f>
+        <v>Profesor Investigador Titular "A"</v>
       </c>
     </row>
     <row r="11">
@@ -858,12 +1027,16 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="3" t="str">
-        <f>CONCATENATE('Hoja 1'!B11, " ", 'Hoja 1'!C11)</f>
-        <v>Mtra. Patricia del Rosario Retamoza Vega</v>
-      </c>
-      <c r="C11" s="2" t="str">
-        <f>'Hoja 1'!E11</f>
-        <v>Profesor de Tiempo Completo Asociado "C"</v>
+        <f>CONCATENATE(Capturando!B11, " ", Capturando!C11, " ", Capturando!D11)</f>
+        <v>Dra. Meda Campaña María Elena</v>
+      </c>
+      <c r="C11" s="13" t="str">
+        <f>Capturando!E11</f>
+        <v>https://mti.cucea.udg.mx/?q=dra-maria-elena-meda-campana#overlay-context=dra-ma-del-rocio-maciel-arellano%3Fq%3Ddra-ma-del-rocio-maciel-arellano</v>
+      </c>
+      <c r="D11" s="2" t="str">
+        <f>Capturando!F11</f>
+        <v>Profesor Investigador Titular "C"</v>
       </c>
     </row>
     <row r="12">
@@ -871,12 +1044,16 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="3" t="str">
-        <f>CONCATENATE('Hoja 1'!B12, " ", 'Hoja 1'!C12)</f>
-        <v>Mtro. Pedro Aguilar Pérez</v>
-      </c>
-      <c r="C12" s="2" t="str">
-        <f>'Hoja 1'!E12</f>
-        <v>Profesor Asistente "B"</v>
+        <f>CONCATENATE(Capturando!B12, " ", Capturando!C12, " ", Capturando!D12)</f>
+        <v>Mtro. Morales Montelongo José Guadalupe</v>
+      </c>
+      <c r="C12" s="13" t="str">
+        <f>Capturando!E12</f>
+        <v>https://mti.cucea.udg.mx/?q=mtro-jose-guadalupe-morales-montelongo#overlay-context=mtro-hugo-enrique-torres-ruvalcaba%3Fq%3Dmtro-hugo-enrique-torres-ruvalcaba</v>
+      </c>
+      <c r="D12" s="2" t="str">
+        <f>Capturando!F12</f>
+        <v>Profesor Titular "A"</v>
       </c>
     </row>
     <row r="13">
@@ -884,12 +1061,16 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="3" t="str">
-        <f>CONCATENATE('Hoja 1'!B13, " ", 'Hoja 1'!C13)</f>
-        <v>Dr. Sergio Roberto Dávalos García</v>
-      </c>
-      <c r="C13" s="2" t="str">
-        <f>'Hoja 1'!E13</f>
-        <v>Profesor Investigador Asociado "A"</v>
+        <f>CONCATENATE(Capturando!B13, " ", Capturando!C13, " ", Capturando!D13)</f>
+        <v>Mtra. Retamoza Vega Patricia del Rosario</v>
+      </c>
+      <c r="C13" s="12" t="str">
+        <f>Capturando!E13</f>
+        <v/>
+      </c>
+      <c r="D13" s="2" t="str">
+        <f>Capturando!F13</f>
+        <v>Profesor de Tiempo Completo Asociado "C"</v>
       </c>
     </row>
     <row r="14">
@@ -897,12 +1078,16 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="3" t="str">
-        <f>CONCATENATE('Hoja 1'!B14, " ", 'Hoja 1'!C14)</f>
-        <v>Mtro. Torres Ruvalcaba Hugo Enrique</v>
-      </c>
-      <c r="C14" s="2" t="str">
-        <f>'Hoja 1'!E14</f>
-        <v>Profesor Asignatura "B"</v>
+        <f>CONCATENATE(Capturando!B14, " ", Capturando!C14, " ", Capturando!D14)</f>
+        <v>Dra. Reynoso Gómez Blanca Lorena</v>
+      </c>
+      <c r="C14" s="13" t="str">
+        <f>Capturando!E14</f>
+        <v>https://mti.cucea.udg.mx/?q=dra-blanca-lorena-reynoso-gomez#overlay-context=practica%3Fq%3Dpractica</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <f>Capturando!F14</f>
+        <v>Profesor Docente Asociado "B"</v>
       </c>
     </row>
     <row r="15">
@@ -910,11 +1095,15 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="3" t="str">
-        <f>CONCATENATE('Hoja 1'!B15, " ", 'Hoja 1'!C15)</f>
-        <v> </v>
-      </c>
-      <c r="C15" s="2" t="str">
-        <f>'Hoja 1'!E15</f>
+        <f>CONCATENATE(Capturando!B15, " ", Capturando!C15, " ", Capturando!D15)</f>
+        <v>  </v>
+      </c>
+      <c r="C15" s="12" t="str">
+        <f>Capturando!E15</f>
+        <v/>
+      </c>
+      <c r="D15" s="2" t="str">
+        <f>Capturando!F15</f>
         <v/>
       </c>
     </row>
@@ -923,11 +1112,15 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="3" t="str">
-        <f>CONCATENATE('Hoja 1'!B16, " ", 'Hoja 1'!C16)</f>
-        <v> </v>
-      </c>
-      <c r="C16" s="2" t="str">
-        <f>'Hoja 1'!E16</f>
+        <f>CONCATENATE(Capturando!B16, " ", Capturando!C16, " ", Capturando!D16)</f>
+        <v>  </v>
+      </c>
+      <c r="C16" s="12" t="str">
+        <f>Capturando!E16</f>
+        <v/>
+      </c>
+      <c r="D16" s="2" t="str">
+        <f>Capturando!F16</f>
         <v/>
       </c>
     </row>
@@ -936,11 +1129,15 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="3" t="str">
-        <f>CONCATENATE('Hoja 1'!B17, " ", 'Hoja 1'!C17)</f>
-        <v> </v>
-      </c>
-      <c r="C17" s="2" t="str">
-        <f>'Hoja 1'!E17</f>
+        <f>CONCATENATE(Capturando!B17, " ", Capturando!C17, " ", Capturando!D17)</f>
+        <v>  </v>
+      </c>
+      <c r="C17" s="12" t="str">
+        <f>Capturando!E17</f>
+        <v/>
+      </c>
+      <c r="D17" s="2" t="str">
+        <f>Capturando!F17</f>
         <v/>
       </c>
     </row>
@@ -949,11 +1146,15 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="3" t="str">
-        <f>CONCATENATE('Hoja 1'!B18, " ", 'Hoja 1'!C18)</f>
-        <v> </v>
-      </c>
-      <c r="C18" s="2" t="str">
-        <f>'Hoja 1'!E18</f>
+        <f>CONCATENATE(Capturando!B18, " ", Capturando!C18, " ", Capturando!D18)</f>
+        <v>  </v>
+      </c>
+      <c r="C18" s="12" t="str">
+        <f>Capturando!E18</f>
+        <v/>
+      </c>
+      <c r="D18" s="2" t="str">
+        <f>Capturando!F18</f>
         <v/>
       </c>
     </row>
@@ -962,11 +1163,15 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="3" t="str">
-        <f>CONCATENATE('Hoja 1'!B19, " ", 'Hoja 1'!C19)</f>
-        <v> </v>
-      </c>
-      <c r="C19" s="2" t="str">
-        <f>'Hoja 1'!E19</f>
+        <f>CONCATENATE(Capturando!B19, " ", Capturando!C19, " ", Capturando!D19)</f>
+        <v>  </v>
+      </c>
+      <c r="C19" s="12" t="str">
+        <f>Capturando!E19</f>
+        <v/>
+      </c>
+      <c r="D19" s="2" t="str">
+        <f>Capturando!F19</f>
         <v/>
       </c>
     </row>
@@ -975,11 +1180,15 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="3" t="str">
-        <f>CONCATENATE('Hoja 1'!B20, " ", 'Hoja 1'!C20)</f>
-        <v> </v>
-      </c>
-      <c r="C20" s="2" t="str">
-        <f>'Hoja 1'!E20</f>
+        <f>CONCATENATE(Capturando!B20, " ", Capturando!C20, " ", Capturando!D20)</f>
+        <v>  </v>
+      </c>
+      <c r="C20" s="12" t="str">
+        <f>Capturando!E20</f>
+        <v/>
+      </c>
+      <c r="D20" s="2" t="str">
+        <f>Capturando!F20</f>
         <v/>
       </c>
     </row>
@@ -988,11 +1197,15 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="3" t="str">
-        <f>CONCATENATE('Hoja 1'!B21, " ", 'Hoja 1'!C21)</f>
-        <v> </v>
-      </c>
-      <c r="C21" s="2" t="str">
-        <f>'Hoja 1'!E21</f>
+        <f>CONCATENATE(Capturando!B21, " ", Capturando!C21, " ", Capturando!D21)</f>
+        <v>  </v>
+      </c>
+      <c r="C21" s="12" t="str">
+        <f>Capturando!E21</f>
+        <v/>
+      </c>
+      <c r="D21" s="2" t="str">
+        <f>Capturando!F21</f>
         <v/>
       </c>
     </row>
@@ -1001,11 +1214,15 @@
         <v>21.0</v>
       </c>
       <c r="B22" s="3" t="str">
-        <f>CONCATENATE('Hoja 1'!B22, " ", 'Hoja 1'!C22)</f>
-        <v> </v>
-      </c>
-      <c r="C22" s="2" t="str">
-        <f>'Hoja 1'!E22</f>
+        <f>CONCATENATE(Capturando!B22, " ", Capturando!C22, " ", Capturando!D22)</f>
+        <v>  </v>
+      </c>
+      <c r="C22" s="12" t="str">
+        <f>Capturando!E22</f>
+        <v/>
+      </c>
+      <c r="D22" s="2" t="str">
+        <f>Capturando!F22</f>
         <v/>
       </c>
     </row>
@@ -1014,11 +1231,15 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="3" t="str">
-        <f>CONCATENATE('Hoja 1'!B23, " ", 'Hoja 1'!C23)</f>
-        <v> </v>
-      </c>
-      <c r="C23" s="2" t="str">
-        <f>'Hoja 1'!E23</f>
+        <f>CONCATENATE(Capturando!B23, " ", Capturando!C23, " ", Capturando!D23)</f>
+        <v>  </v>
+      </c>
+      <c r="C23" s="12" t="str">
+        <f>Capturando!E23</f>
+        <v/>
+      </c>
+      <c r="D23" s="2" t="str">
+        <f>Capturando!F23</f>
         <v/>
       </c>
     </row>

</xml_diff>